<commit_message>
2015-08-12 11:43 UTC--300 NaldoDj (marinaldo/dot/jesus/at/blacktdn/dot/com)
</commit_message>
<xml_diff>
--- a/templates/office/excel/rh/pensao/CalculoPensao.xlsx
+++ b/templates/office/excel/rh/pensao/CalculoPensao.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="75" windowWidth="13530" windowHeight="8175" activeTab="2"/>
+    <workbookView xWindow="255" yWindow="75" windowWidth="13530" windowHeight="8175"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionários" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
@@ -244,6 +244,11 @@
       <name val="Cambria"/>
       <family val="1"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -553,7 +558,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -693,12 +698,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -816,6 +815,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="8" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -826,6 +848,80 @@
     <cellStyle name="Paystub Style 1" xfId="4"/>
   </cellStyles>
   <dxfs count="69">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2340,77 +2436,7 @@
           <color auto="1"/>
         </horizontal>
       </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2883,58 +2909,58 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A1:G5" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:G5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A1:G7" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:G7"/>
   <tableColumns count="7">
     <tableColumn id="1" name="ID" dataDxfId="52" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Funcionário" dataDxfId="51" dataCellStyle="Normal">
-      <calculatedColumnFormula>VLOOKUP(A2,Funcionários!$A$2:$C$2,2,FALSE)</calculatedColumnFormula>
+    <tableColumn id="2" name="Funcionário" dataDxfId="0" dataCellStyle="Normal">
+      <calculatedColumnFormula>VLOOKUP(A2,Funcionários!A:B,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento" dataDxfId="50" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Descrição" dataDxfId="49" dataCellStyle="Normal">
-      <calculatedColumnFormula>VLOOKUP(C2,Eventos!A2:B11,2,FALSE)</calculatedColumnFormula>
+    <tableColumn id="3" name="Evento" dataDxfId="51" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Descrição" dataDxfId="1" dataCellStyle="Normal">
+      <calculatedColumnFormula>VLOOKUP(C2,Eventos!A:B,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Valor" dataDxfId="48" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="IRRF" dataDxfId="47" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="Pensao" dataDxfId="46" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Valor" dataDxfId="50" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="IRRF" dataDxfId="49" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="Pensao" dataDxfId="48" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="Payroll Calculator" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K2" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K2" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:K2"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID" dataDxfId="43" totalsRowDxfId="42" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Funcionário" dataDxfId="41" totalsRowDxfId="40" dataCellStyle="Normal">
-      <calculatedColumnFormula>VLOOKUP(A2,Funcionários!$A$2:$C$2,2,FALSE)</calculatedColumnFormula>
+    <tableColumn id="1" name="ID" dataDxfId="45" totalsRowDxfId="44" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Funcionário" dataDxfId="43" totalsRowDxfId="42" dataCellStyle="Normal">
+      <calculatedColumnFormula>VLOOKUP(A2,Funcionários!A:B,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Somar Base IRRF" dataDxfId="39" totalsRowDxfId="38">
+    <tableColumn id="3" name="Somar Base IRRF" dataDxfId="41" totalsRowDxfId="40">
       <calculatedColumnFormula>SUMIFS(Table27[Valor],Table27[ID],Table1[ID],Table27[IRRF],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Base IRRF" dataDxfId="37" totalsRowDxfId="36">
+    <tableColumn id="11" name="Base IRRF" dataDxfId="39" totalsRowDxfId="38">
       <calculatedColumnFormula>Table2[Somar Base IRRF]-Table2[Pensão]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% IRRF" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="12" name="% IRRF" dataDxfId="37" totalsRowDxfId="36">
       <calculatedColumnFormula>VLOOKUP(Table2[Base IRRF],Tabela9[[Faixa Inicial]:[Alíquota (%)]],3,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Dedução" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="18" name="Dedução" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>VLOOKUP(Table2[Base IRRF],Tabela11[[Faixa Inicial]:[Parcela a Deduzir]],3,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="IRRF" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="19" name="IRRF" dataDxfId="33" totalsRowDxfId="32">
       <calculatedColumnFormula>Table2[Base IRRF]*Table2[% IRRF]-Table2[Dedução]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Somar Base Pensão" dataDxfId="29" totalsRowDxfId="28" dataCellStyle="Normal">
+    <tableColumn id="5" name="Somar Base Pensão" dataDxfId="31" totalsRowDxfId="30" dataCellStyle="Normal">
       <calculatedColumnFormula>SUMIFS(Table27[Valor],Table27[ID],Table1[ID],Table27[Pensao],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Base Pensão" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="21" name="Base Pensão" dataDxfId="29" totalsRowDxfId="28">
       <calculatedColumnFormula>Table2[Somar Base Pensão]-Table2[IRRF]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="% Pensão" dataDxfId="25" totalsRowDxfId="24">
-      <calculatedColumnFormula>Table1[% Pensao]</calculatedColumnFormula>
+    <tableColumn id="20" name="% Pensão" dataDxfId="27" totalsRowDxfId="26">
+      <calculatedColumnFormula>VLOOKUP(A2,Funcionários!A:C,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Pensão" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="13" name="Pensão" dataDxfId="25" totalsRowDxfId="24">
       <calculatedColumnFormula>Table2[Base Pensão]*Table2[% Pensão]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2943,41 +2969,41 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela9" displayName="Tabela9" ref="A1:D6" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela9" displayName="Tabela9" ref="A1:D6" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A1:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Faixa" dataDxfId="16"/>
-    <tableColumn id="2" name="Faixa Inicial" dataDxfId="15">
+    <tableColumn id="1" name="Faixa" dataDxfId="18"/>
+    <tableColumn id="2" name="Faixa Inicial" dataDxfId="17">
       <calculatedColumnFormula>C1+0.01</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Faixa Final" dataDxfId="14"/>
-    <tableColumn id="4" name="Alíquota (%)" dataDxfId="13"/>
+    <tableColumn id="3" name="Faixa Final" dataDxfId="16"/>
+    <tableColumn id="4" name="Alíquota (%)" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabela11" displayName="Tabela11" ref="A8:D13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabela11" displayName="Tabela11" ref="A8:D13" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A8:D13"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Faixa" dataDxfId="7"/>
-    <tableColumn id="2" name="Faixa Inicial" dataDxfId="6">
+    <tableColumn id="1" name="Faixa" dataDxfId="9"/>
+    <tableColumn id="2" name="Faixa Inicial" dataDxfId="8">
       <calculatedColumnFormula>B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Faixa Final" dataDxfId="5"/>
-    <tableColumn id="4" name="Parcela a Deduzir" dataDxfId="4"/>
+    <tableColumn id="3" name="Faixa Final" dataDxfId="7"/>
+    <tableColumn id="4" name="Parcela a Deduzir" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2456" displayName="Table2456" ref="A1:B4" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2456" displayName="Table2456" ref="A1:B4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Evento" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Descrição" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Evento" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Descrição" dataDxfId="2" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="Payroll Calculator" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3317,39 +3343,39 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="246" width="12" style="56" customWidth="1"/>
-    <col min="247" max="16384" width="9.33203125" style="56"/>
+    <col min="1" max="1" width="6.1640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="246" width="12" style="54" customWidth="1"/>
+    <col min="247" max="16384" width="9.33203125" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:3" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="52" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="49">
+      <c r="A2" s="47">
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="49">
         <v>0.23</v>
       </c>
     </row>
@@ -3392,26 +3418,26 @@
   <sheetPr codeName="Plan2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="60" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="65" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="60" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="62" bestFit="1" customWidth="1"/>
-    <col min="7" max="245" width="12" style="62" customWidth="1"/>
-    <col min="246" max="16384" width="9.33203125" style="62"/>
+    <col min="1" max="1" width="7.1640625" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="63" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="245" width="12" style="60" customWidth="1"/>
+    <col min="246" max="16384" width="9.33203125" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:7" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="37" t="s">
@@ -3423,29 +3449,29 @@
       <c r="D1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="27">
         <v>1</v>
       </c>
       <c r="B2" s="38" t="str">
-        <f>VLOOKUP(A2,Funcionários!$A$2:$C$2,2,FALSE)</f>
+        <f>VLOOKUP(A2,Funcionários!A:B,2,FALSE)</f>
         <v>Nome do Funcionário 1</v>
       </c>
       <c r="C2" s="28">
         <v>1</v>
       </c>
       <c r="D2" s="38" t="str">
-        <f>VLOOKUP(C2,Eventos!A2:B11,2,FALSE)</f>
+        <f>VLOOKUP(C2,Eventos!A:B,2,FALSE)</f>
         <v>Salário Base</v>
       </c>
       <c r="E2" s="29">
@@ -3458,18 +3484,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27">
         <v>1</v>
       </c>
-      <c r="B3" s="39" t="str">
-        <f>VLOOKUP(A3,Funcionários!$A$2:$C$2,2,FALSE)</f>
+      <c r="B3" s="38" t="str">
+        <f>VLOOKUP(A3,Funcionários!A:B,2,FALSE)</f>
         <v>Nome do Funcionário 1</v>
       </c>
       <c r="C3" s="32">
         <v>2</v>
       </c>
-      <c r="D3" s="39" t="str">
+      <c r="D3" s="38" t="str">
         <f>VLOOKUP(C3,Eventos!A:B,2,FALSE)</f>
         <v>Anuênio</v>
       </c>
@@ -3483,461 +3509,511 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27">
+    <row r="4" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="72">
         <v>1</v>
       </c>
       <c r="B4" s="38" t="str">
-        <f>VLOOKUP(A4,Funcionários!$A$2:$C$2,2,FALSE)</f>
+        <f>VLOOKUP(A4,Funcionários!A:B,2,FALSE)</f>
         <v>Nome do Funcionário 1</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="74">
+        <v>3</v>
+      </c>
+      <c r="D4" s="73" t="str">
+        <f>VLOOKUP(C4,Eventos!A:B,2,FALSE)</f>
+        <v>HE 50%</v>
+      </c>
+      <c r="E4" s="75">
+        <v>500</v>
+      </c>
+      <c r="F4" s="76">
+        <v>1</v>
+      </c>
+      <c r="G4" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="72">
+        <v>1</v>
+      </c>
+      <c r="B5" s="38" t="str">
+        <f>VLOOKUP(A5,Funcionários!A:B,2,FALSE)</f>
+        <v>Nome do Funcionário 1</v>
+      </c>
+      <c r="C5" s="74">
+        <v>4</v>
+      </c>
+      <c r="D5" s="73" t="str">
+        <f>VLOOKUP(C5,Eventos!A:B,2,FALSE)</f>
+        <v>HE 100%</v>
+      </c>
+      <c r="E5" s="75">
+        <v>1500</v>
+      </c>
+      <c r="F5" s="76">
+        <v>1</v>
+      </c>
+      <c r="G5" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27">
+        <v>1</v>
+      </c>
+      <c r="B6" s="38" t="str">
+        <f>VLOOKUP(A6,Funcionários!A:B,2,FALSE)</f>
+        <v>Nome do Funcionário 1</v>
+      </c>
+      <c r="C6" s="28">
         <v>10</v>
       </c>
-      <c r="D4" s="39" t="str">
-        <f>VLOOKUP(C4,Eventos!A:B,2,FALSE)</f>
+      <c r="D6" s="38" t="str">
+        <f>VLOOKUP(C6,Eventos!A:B,2,FALSE)</f>
         <v>Previdência Privada</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E6" s="29">
         <v>-78.12</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F6" s="30">
         <v>1</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G6" s="31">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27">
+    <row r="7" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27">
         <v>1</v>
       </c>
-      <c r="B5" s="40" t="str">
-        <f>VLOOKUP(A5,Funcionários!$A$2:$C$2,2,FALSE)</f>
+      <c r="B7" s="38" t="str">
+        <f>VLOOKUP(A7,Funcionários!A:B,2,FALSE)</f>
         <v>Nome do Funcionário 1</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C7" s="33">
         <v>5</v>
       </c>
-      <c r="D5" s="40" t="str">
-        <f>VLOOKUP(C5,Eventos!A5:B14,2,FALSE)</f>
+      <c r="D7" s="38" t="str">
+        <f>VLOOKUP(C7,Eventos!A:B,2,FALSE)</f>
         <v>INSS</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E7" s="34">
         <v>-363</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F7" s="35">
         <v>1</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G7" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
-      <c r="B8" s="63"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="63"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
-      <c r="B9" s="63"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="63"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
-      <c r="B10" s="63"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="63"/>
+      <c r="D10" s="61"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
-      <c r="B11" s="63"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="63"/>
+      <c r="D11" s="61"/>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
-      <c r="B12" s="63"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="63"/>
+      <c r="D12" s="61"/>
       <c r="E12" s="13"/>
     </row>
-    <row r="13" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="63"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="63"/>
+      <c r="D13" s="61"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
-      <c r="B14" s="63"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="13"/>
-      <c r="D14" s="63"/>
+      <c r="D14" s="61"/>
       <c r="E14" s="13"/>
     </row>
-    <row r="15" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
-      <c r="B15" s="63"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="13"/>
-      <c r="D15" s="63"/>
+      <c r="D15" s="61"/>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" spans="1:7" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="63"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="63"/>
+      <c r="D16" s="61"/>
       <c r="E16" s="13"/>
     </row>
-    <row r="17" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
-      <c r="B17" s="63"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="63"/>
+      <c r="D17" s="61"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-    </row>
-    <row r="18" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
-      <c r="B18" s="63"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="63"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-    </row>
-    <row r="19" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="63"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="63"/>
+      <c r="D19" s="61"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-    </row>
-    <row r="20" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+    </row>
+    <row r="20" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
-      <c r="B20" s="63"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="63"/>
+      <c r="D20" s="61"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-    </row>
-    <row r="21" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+    </row>
+    <row r="21" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
-      <c r="B21" s="63"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="63"/>
+      <c r="D21" s="61"/>
       <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+    </row>
+    <row r="22" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
-      <c r="B22" s="63"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="63"/>
+      <c r="D22" s="61"/>
       <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+    </row>
+    <row r="23" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
-      <c r="B23" s="63"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="63"/>
+      <c r="D23" s="61"/>
       <c r="E23" s="13"/>
     </row>
-    <row r="24" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
-      <c r="B24" s="63"/>
+      <c r="B24" s="61"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="63"/>
+      <c r="D24" s="61"/>
       <c r="E24" s="13"/>
     </row>
-    <row r="25" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
-      <c r="B25" s="63"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="63"/>
+      <c r="D25" s="61"/>
       <c r="E25" s="13"/>
     </row>
-    <row r="26" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
-      <c r="B26" s="63"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="63"/>
+      <c r="D26" s="61"/>
       <c r="E26" s="13"/>
     </row>
-    <row r="27" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
-      <c r="B27" s="63"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="63"/>
+      <c r="D27" s="61"/>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
-      <c r="B28" s="63"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="63"/>
+      <c r="D28" s="61"/>
       <c r="E28" s="13"/>
     </row>
-    <row r="29" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
-      <c r="B29" s="63"/>
+      <c r="B29" s="61"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="63"/>
+      <c r="D29" s="61"/>
       <c r="E29" s="13"/>
     </row>
-    <row r="30" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
-      <c r="B30" s="63"/>
+      <c r="B30" s="61"/>
       <c r="C30" s="13"/>
-      <c r="D30" s="63"/>
+      <c r="D30" s="61"/>
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
-      <c r="B31" s="63"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="13"/>
-      <c r="D31" s="63"/>
+      <c r="D31" s="61"/>
       <c r="E31" s="13"/>
     </row>
-    <row r="32" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
-      <c r="B32" s="63"/>
+      <c r="B32" s="61"/>
       <c r="C32" s="13"/>
-      <c r="D32" s="63"/>
+      <c r="D32" s="61"/>
       <c r="E32" s="13"/>
     </row>
-    <row r="33" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
-      <c r="B33" s="63"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="13"/>
-      <c r="D33" s="63"/>
+      <c r="D33" s="61"/>
       <c r="E33" s="13"/>
     </row>
-    <row r="34" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
-      <c r="B34" s="63"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="13"/>
-      <c r="D34" s="63"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="13"/>
     </row>
-    <row r="35" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
-      <c r="B35" s="63"/>
+      <c r="B35" s="61"/>
       <c r="C35" s="13"/>
-      <c r="D35" s="63"/>
+      <c r="D35" s="61"/>
       <c r="E35" s="13"/>
     </row>
-    <row r="36" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="61"/>
-    </row>
-    <row r="37" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="61"/>
-    </row>
-    <row r="38" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="60"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="61"/>
-    </row>
-    <row r="39" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="60"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="61"/>
-    </row>
-    <row r="40" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="60"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="61"/>
-    </row>
-    <row r="41" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="60"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="61"/>
-    </row>
-    <row r="42" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="60"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="61"/>
-    </row>
-    <row r="43" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="60"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="61"/>
-    </row>
-    <row r="44" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="60"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="61"/>
-    </row>
-    <row r="45" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="60"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="61"/>
-    </row>
-    <row r="46" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="60"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="61"/>
-    </row>
-    <row r="47" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="60"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="61"/>
-    </row>
-    <row r="48" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="60"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="61"/>
-    </row>
-    <row r="49" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="60"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="61"/>
-    </row>
-    <row r="50" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="60"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="61"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="61"/>
-    </row>
-    <row r="51" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="60"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="61"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="61"/>
-    </row>
-    <row r="52" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="60"/>
-      <c r="B52" s="64"/>
-      <c r="C52" s="61"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="61"/>
-    </row>
-    <row r="53" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="60"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="61"/>
-    </row>
-    <row r="54" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="60"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="61"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="61"/>
-    </row>
-    <row r="55" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="60"/>
-      <c r="B55" s="64"/>
-      <c r="C55" s="61"/>
-      <c r="D55" s="64"/>
-      <c r="E55" s="61"/>
-    </row>
-    <row r="56" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="60"/>
-      <c r="B56" s="64"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="61"/>
-    </row>
-    <row r="57" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="60"/>
-      <c r="B57" s="64"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="64"/>
-      <c r="E57" s="61"/>
-    </row>
-    <row r="58" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="60"/>
-      <c r="B58" s="64"/>
-      <c r="C58" s="61"/>
-      <c r="D58" s="64"/>
-      <c r="E58" s="61"/>
-    </row>
-    <row r="59" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="60"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="61"/>
-      <c r="D59" s="64"/>
-      <c r="E59" s="61"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B60" s="64"/>
-      <c r="C60" s="61"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="59"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F61" s="59"/>
-      <c r="G61" s="59"/>
+    <row r="36" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="13"/>
+    </row>
+    <row r="38" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="58"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="59"/>
+    </row>
+    <row r="39" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="58"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="59"/>
+    </row>
+    <row r="40" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="58"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="59"/>
+    </row>
+    <row r="41" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="58"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="59"/>
+    </row>
+    <row r="42" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="58"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="59"/>
+    </row>
+    <row r="43" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="58"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="59"/>
+    </row>
+    <row r="44" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="58"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="59"/>
+    </row>
+    <row r="45" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="58"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="59"/>
+    </row>
+    <row r="46" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="58"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="59"/>
+    </row>
+    <row r="47" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="58"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="59"/>
+    </row>
+    <row r="48" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="58"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="59"/>
+    </row>
+    <row r="49" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="58"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="59"/>
+    </row>
+    <row r="50" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="58"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="59"/>
+    </row>
+    <row r="51" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="58"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="59"/>
+    </row>
+    <row r="52" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="58"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="59"/>
+    </row>
+    <row r="53" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="58"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="59"/>
+    </row>
+    <row r="54" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="58"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="62"/>
+      <c r="E54" s="59"/>
+    </row>
+    <row r="55" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="58"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="62"/>
+      <c r="E55" s="59"/>
+    </row>
+    <row r="56" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="58"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="62"/>
+      <c r="E56" s="59"/>
+    </row>
+    <row r="57" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="58"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="59"/>
+    </row>
+    <row r="58" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="58"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="62"/>
+      <c r="E58" s="59"/>
+    </row>
+    <row r="59" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="58"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="59"/>
+    </row>
+    <row r="60" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="58"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="59"/>
+    </row>
+    <row r="61" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="58"/>
+      <c r="B61" s="62"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="59"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F62" s="59"/>
-      <c r="G62" s="59"/>
+      <c r="B62" s="62"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="62"/>
+      <c r="E62" s="59"/>
+      <c r="F62" s="57"/>
+      <c r="G62" s="57"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F63" s="59"/>
-      <c r="G63" s="59"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="57"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F64" s="57"/>
+      <c r="G64" s="57"/>
+    </row>
+    <row r="65" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F65" s="57"/>
+      <c r="G65" s="57"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" insertRows="0" deleteRows="0" autoFilter="0"/>
@@ -3945,9 +4021,6 @@
   <pageMargins left="0.6" right="0.6" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="D3 D4" calculatedColumn="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -3961,32 +4034,32 @@
   </sheetPr>
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" style="65" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="65" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="65" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="65" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="65" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" style="73" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" style="73" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="73" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" style="60" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="60" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="60" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" style="56"/>
-    <col min="16" max="260" width="12" style="62" customWidth="1"/>
-    <col min="261" max="16384" width="9.33203125" style="62"/>
+    <col min="1" max="1" width="7.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="63" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="63" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="63" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" style="71" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" style="71" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="71" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="71" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" style="58" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="58" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="54"/>
+    <col min="16" max="260" width="12" style="60" customWidth="1"/>
+    <col min="261" max="16384" width="9.33203125" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="67" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="65" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
@@ -4020,1029 +4093,1029 @@
       <c r="K1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="66"/>
-    </row>
-    <row r="2" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="64"/>
+    </row>
+    <row r="2" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23">
         <v>1</v>
       </c>
       <c r="B2" s="26" t="str">
-        <f>VLOOKUP(A2,Funcionários!$A$2:$C$2,2,FALSE)</f>
+        <f>VLOOKUP(A2,Funcionários!A:B,2,FALSE)</f>
         <v>Nome do Funcionário 1</v>
       </c>
       <c r="C2" s="26">
         <f>SUMIFS(Table27[Valor],Table27[ID],Table1[ID],Table27[IRRF],1)</f>
-        <v>2858.88</v>
+        <v>4858.88</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">Table2[Somar Base IRRF]-Table2[Pensão]</f>
-        <v>2188.2737216993132</v>
+        <v>3772.2753493277091</v>
       </c>
       <c r="E2" s="2">
         <f ca="1">VLOOKUP(Table2[Base IRRF],Tabela9[[Faixa Inicial]:[Alíquota (%)]],3,TRUE)</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="F2" s="1">
         <f ca="1">VLOOKUP(Table2[Base IRRF],Tabela11[[Faixa Inicial]:[Parcela a Deduzir]],3,TRUE)</f>
-        <v>142.80000000000001</v>
+        <v>636.13</v>
       </c>
       <c r="G2" s="1">
         <f ca="1">Table2[Base IRRF]*Table2[% IRRF]-Table2[Dedução]</f>
-        <v>21.320529127448481</v>
+        <v>212.63195359873453</v>
       </c>
       <c r="H2" s="1">
         <f>SUMIFS(Table27[Valor],Table27[ID],Table1[ID],Table27[Pensao],1)</f>
-        <v>2937</v>
+        <v>4937</v>
       </c>
       <c r="I2" s="1">
         <f ca="1">Table2[Somar Base Pensão]-Table2[IRRF]</f>
-        <v>2915.6794708725515</v>
+        <v>4724.368046401265</v>
       </c>
       <c r="J2" s="2">
-        <f>Table1[% Pensao]</f>
+        <f>VLOOKUP(A2,Funcionários!A:C,3,FALSE)</f>
         <v>0.23</v>
       </c>
       <c r="K2" s="1">
         <f ca="1">Table2[Base Pensão]*Table2[% Pensão]</f>
-        <v>670.60627830068688</v>
-      </c>
-      <c r="L2" s="68"/>
-    </row>
-    <row r="3" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+        <v>1086.604650672291</v>
+      </c>
+      <c r="L2" s="66"/>
+    </row>
+    <row r="3" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="67"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="69"/>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+    <row r="4" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="67"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="69"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
+    <row r="5" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="67"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="69"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
+    <row r="6" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="67"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
     </row>
-    <row r="8" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
     </row>
-    <row r="10" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
     </row>
-    <row r="11" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
     </row>
-    <row r="12" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
     </row>
-    <row r="14" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
     </row>
-    <row r="16" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
     </row>
-    <row r="17" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="69"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
     </row>
-    <row r="18" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="71"/>
-      <c r="K19" s="71"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
     </row>
-    <row r="20" spans="1:14" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
     </row>
-    <row r="21" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
     </row>
-    <row r="22" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
       <c r="N22" s="13"/>
     </row>
-    <row r="23" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="70"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
     </row>
-    <row r="24" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="72"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>
     </row>
-    <row r="25" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="72"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="70"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
     </row>
-    <row r="26" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
     </row>
-    <row r="27" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="72"/>
-      <c r="K27" s="72"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="72"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
     </row>
-    <row r="29" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72"/>
-      <c r="K29" s="72"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="70"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
     </row>
-    <row r="30" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
-      <c r="K30" s="72"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="70"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="72"/>
-      <c r="I31" s="72"/>
-      <c r="J31" s="72"/>
-      <c r="K31" s="72"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
     </row>
-    <row r="32" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="72"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
     </row>
-    <row r="33" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
-      <c r="K33" s="72"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
       <c r="L33" s="13"/>
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
     </row>
-    <row r="34" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="72"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
     </row>
-    <row r="35" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="72"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="72"/>
-      <c r="K35" s="72"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="70"/>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
     </row>
-    <row r="36" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="61"/>
-      <c r="M36" s="61"/>
-      <c r="N36" s="61"/>
-    </row>
-    <row r="37" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="61"/>
-    </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="60"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="64"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="61"/>
-    </row>
-    <row r="39" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="60"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="61"/>
-    </row>
-    <row r="40" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="60"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="61"/>
-    </row>
-    <row r="41" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="60"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="72"/>
-      <c r="K41" s="72"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="61"/>
-      <c r="N41" s="61"/>
-    </row>
-    <row r="42" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="60"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
-      <c r="F42" s="64"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="61"/>
-      <c r="M42" s="61"/>
-      <c r="N42" s="61"/>
-    </row>
-    <row r="43" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="60"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="72"/>
-      <c r="L43" s="61"/>
-      <c r="M43" s="61"/>
-      <c r="N43" s="61"/>
-    </row>
-    <row r="44" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="60"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="72"/>
-      <c r="I44" s="72"/>
-      <c r="J44" s="72"/>
-      <c r="K44" s="72"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="61"/>
-      <c r="N44" s="61"/>
-    </row>
-    <row r="45" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="60"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="72"/>
-      <c r="K45" s="72"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="61"/>
-      <c r="N45" s="61"/>
-    </row>
-    <row r="46" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="60"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="72"/>
-      <c r="J46" s="72"/>
-      <c r="K46" s="72"/>
-      <c r="L46" s="61"/>
-      <c r="M46" s="61"/>
-      <c r="N46" s="61"/>
-    </row>
-    <row r="47" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="60"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="72"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="72"/>
-      <c r="L47" s="61"/>
-      <c r="M47" s="61"/>
-      <c r="N47" s="61"/>
-    </row>
-    <row r="48" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="60"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="72"/>
-      <c r="I48" s="72"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="72"/>
-      <c r="L48" s="61"/>
-      <c r="M48" s="61"/>
-      <c r="N48" s="61"/>
-    </row>
-    <row r="49" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="60"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="72"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="72"/>
-      <c r="K49" s="72"/>
-      <c r="L49" s="61"/>
-      <c r="M49" s="61"/>
-      <c r="N49" s="61"/>
-    </row>
-    <row r="50" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="60"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="72"/>
-      <c r="I50" s="72"/>
-      <c r="J50" s="72"/>
-      <c r="K50" s="72"/>
-      <c r="L50" s="61"/>
-      <c r="M50" s="61"/>
-      <c r="N50" s="61"/>
-    </row>
-    <row r="51" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="60"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
-      <c r="K51" s="72"/>
-      <c r="L51" s="61"/>
-      <c r="M51" s="61"/>
-      <c r="N51" s="61"/>
-    </row>
-    <row r="52" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="60"/>
-      <c r="B52" s="64"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="72"/>
-      <c r="K52" s="72"/>
-      <c r="L52" s="61"/>
-      <c r="M52" s="61"/>
-      <c r="N52" s="61"/>
-    </row>
-    <row r="53" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="60"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="64"/>
-      <c r="H53" s="72"/>
-      <c r="I53" s="72"/>
-      <c r="J53" s="72"/>
-      <c r="K53" s="72"/>
-      <c r="L53" s="61"/>
-      <c r="M53" s="61"/>
-      <c r="N53" s="61"/>
-    </row>
-    <row r="54" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="60"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="64"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="64"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="72"/>
-      <c r="K54" s="72"/>
-      <c r="L54" s="61"/>
-      <c r="M54" s="61"/>
-      <c r="N54" s="61"/>
-    </row>
-    <row r="55" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="60"/>
-      <c r="B55" s="64"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="64"/>
-      <c r="E55" s="64"/>
-      <c r="F55" s="64"/>
-      <c r="G55" s="64"/>
-      <c r="H55" s="72"/>
-      <c r="I55" s="72"/>
-      <c r="J55" s="72"/>
-      <c r="K55" s="72"/>
-      <c r="L55" s="61"/>
-      <c r="M55" s="61"/>
-      <c r="N55" s="61"/>
-    </row>
-    <row r="56" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="60"/>
-      <c r="B56" s="64"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="64"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
-      <c r="J56" s="72"/>
-      <c r="K56" s="72"/>
-      <c r="L56" s="61"/>
-      <c r="M56" s="61"/>
-      <c r="N56" s="61"/>
-    </row>
-    <row r="57" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="60"/>
-      <c r="B57" s="64"/>
-      <c r="C57" s="64"/>
-      <c r="D57" s="64"/>
-      <c r="E57" s="64"/>
-      <c r="F57" s="64"/>
-      <c r="G57" s="64"/>
-      <c r="H57" s="72"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="72"/>
-      <c r="K57" s="72"/>
-      <c r="L57" s="61"/>
-      <c r="M57" s="61"/>
-      <c r="N57" s="61"/>
-    </row>
-    <row r="58" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="60"/>
-      <c r="B58" s="64"/>
-      <c r="C58" s="64"/>
-      <c r="D58" s="64"/>
-      <c r="E58" s="64"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="64"/>
-      <c r="H58" s="72"/>
-      <c r="I58" s="72"/>
-      <c r="J58" s="72"/>
-      <c r="K58" s="72"/>
-      <c r="L58" s="61"/>
-      <c r="M58" s="61"/>
-      <c r="N58" s="61"/>
-    </row>
-    <row r="59" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="60"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="64"/>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
-      <c r="F59" s="64"/>
-      <c r="G59" s="64"/>
-      <c r="H59" s="72"/>
-      <c r="I59" s="72"/>
-      <c r="J59" s="72"/>
-      <c r="K59" s="72"/>
-      <c r="L59" s="61"/>
-      <c r="M59" s="61"/>
-      <c r="N59" s="61"/>
-    </row>
-    <row r="60" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="60"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="64"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="64"/>
-      <c r="G60" s="64"/>
-      <c r="H60" s="72"/>
-      <c r="I60" s="72"/>
-      <c r="J60" s="72"/>
-      <c r="K60" s="72"/>
-      <c r="L60" s="61"/>
-      <c r="M60" s="61"/>
-      <c r="N60" s="61"/>
-    </row>
-    <row r="61" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="60"/>
-      <c r="B61" s="65"/>
-      <c r="C61" s="65"/>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65"/>
-      <c r="F61" s="65"/>
-      <c r="G61" s="65"/>
-      <c r="H61" s="72"/>
-      <c r="I61" s="72"/>
-      <c r="J61" s="72"/>
-      <c r="K61" s="72"/>
-      <c r="L61" s="60"/>
-      <c r="M61" s="60"/>
-      <c r="N61" s="60"/>
-    </row>
-    <row r="62" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="60"/>
-      <c r="B62" s="65"/>
-      <c r="C62" s="65"/>
-      <c r="D62" s="65"/>
-      <c r="E62" s="65"/>
-      <c r="F62" s="65"/>
-      <c r="G62" s="65"/>
-      <c r="H62" s="72"/>
-      <c r="I62" s="72"/>
-      <c r="J62" s="72"/>
-      <c r="K62" s="72"/>
-      <c r="L62" s="60"/>
-      <c r="M62" s="60"/>
-      <c r="N62" s="60"/>
-    </row>
-    <row r="63" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="60"/>
-      <c r="B63" s="65"/>
-      <c r="C63" s="65"/>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="65"/>
-      <c r="G63" s="65"/>
-      <c r="H63" s="72"/>
-      <c r="I63" s="72"/>
-      <c r="J63" s="72"/>
-      <c r="K63" s="72"/>
-      <c r="L63" s="60"/>
-      <c r="M63" s="60"/>
-      <c r="N63" s="60"/>
+    <row r="36" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="58"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="59"/>
+      <c r="N36" s="59"/>
+    </row>
+    <row r="37" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="58"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+    </row>
+    <row r="38" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="58"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="59"/>
+      <c r="M38" s="59"/>
+      <c r="N38" s="59"/>
+    </row>
+    <row r="39" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="58"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="59"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="59"/>
+    </row>
+    <row r="40" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="58"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="70"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+    </row>
+    <row r="41" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="58"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="70"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="59"/>
+      <c r="M41" s="59"/>
+      <c r="N41" s="59"/>
+    </row>
+    <row r="42" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="58"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="70"/>
+      <c r="J42" s="70"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+    </row>
+    <row r="43" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="58"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="70"/>
+      <c r="J43" s="70"/>
+      <c r="K43" s="70"/>
+      <c r="L43" s="59"/>
+      <c r="M43" s="59"/>
+      <c r="N43" s="59"/>
+    </row>
+    <row r="44" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="58"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="70"/>
+      <c r="J44" s="70"/>
+      <c r="K44" s="70"/>
+      <c r="L44" s="59"/>
+      <c r="M44" s="59"/>
+      <c r="N44" s="59"/>
+    </row>
+    <row r="45" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="58"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="70"/>
+      <c r="K45" s="70"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+    </row>
+    <row r="46" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="58"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="70"/>
+      <c r="J46" s="70"/>
+      <c r="K46" s="70"/>
+      <c r="L46" s="59"/>
+      <c r="M46" s="59"/>
+      <c r="N46" s="59"/>
+    </row>
+    <row r="47" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="58"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="70"/>
+      <c r="J47" s="70"/>
+      <c r="K47" s="70"/>
+      <c r="L47" s="59"/>
+      <c r="M47" s="59"/>
+      <c r="N47" s="59"/>
+    </row>
+    <row r="48" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="58"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="62"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="70"/>
+      <c r="I48" s="70"/>
+      <c r="J48" s="70"/>
+      <c r="K48" s="70"/>
+      <c r="L48" s="59"/>
+      <c r="M48" s="59"/>
+      <c r="N48" s="59"/>
+    </row>
+    <row r="49" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="58"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="62"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="70"/>
+      <c r="J49" s="70"/>
+      <c r="K49" s="70"/>
+      <c r="L49" s="59"/>
+      <c r="M49" s="59"/>
+      <c r="N49" s="59"/>
+    </row>
+    <row r="50" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="58"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="70"/>
+      <c r="L50" s="59"/>
+      <c r="M50" s="59"/>
+      <c r="N50" s="59"/>
+    </row>
+    <row r="51" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="58"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
+      <c r="J51" s="70"/>
+      <c r="K51" s="70"/>
+      <c r="L51" s="59"/>
+      <c r="M51" s="59"/>
+      <c r="N51" s="59"/>
+    </row>
+    <row r="52" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="58"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
+      <c r="J52" s="70"/>
+      <c r="K52" s="70"/>
+      <c r="L52" s="59"/>
+      <c r="M52" s="59"/>
+      <c r="N52" s="59"/>
+    </row>
+    <row r="53" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="58"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="70"/>
+      <c r="I53" s="70"/>
+      <c r="J53" s="70"/>
+      <c r="K53" s="70"/>
+      <c r="L53" s="59"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="59"/>
+    </row>
+    <row r="54" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="58"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="62"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="62"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="70"/>
+      <c r="J54" s="70"/>
+      <c r="K54" s="70"/>
+      <c r="L54" s="59"/>
+      <c r="M54" s="59"/>
+      <c r="N54" s="59"/>
+    </row>
+    <row r="55" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="58"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="62"/>
+      <c r="E55" s="62"/>
+      <c r="F55" s="62"/>
+      <c r="G55" s="62"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="70"/>
+      <c r="J55" s="70"/>
+      <c r="K55" s="70"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+    </row>
+    <row r="56" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="58"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="62"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="62"/>
+      <c r="G56" s="62"/>
+      <c r="H56" s="70"/>
+      <c r="I56" s="70"/>
+      <c r="J56" s="70"/>
+      <c r="K56" s="70"/>
+      <c r="L56" s="59"/>
+      <c r="M56" s="59"/>
+      <c r="N56" s="59"/>
+    </row>
+    <row r="57" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="58"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="62"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="70"/>
+      <c r="I57" s="70"/>
+      <c r="J57" s="70"/>
+      <c r="K57" s="70"/>
+      <c r="L57" s="59"/>
+      <c r="M57" s="59"/>
+      <c r="N57" s="59"/>
+    </row>
+    <row r="58" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="58"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
+      <c r="E58" s="62"/>
+      <c r="F58" s="62"/>
+      <c r="G58" s="62"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="70"/>
+      <c r="J58" s="70"/>
+      <c r="K58" s="70"/>
+      <c r="L58" s="59"/>
+      <c r="M58" s="59"/>
+      <c r="N58" s="59"/>
+    </row>
+    <row r="59" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="58"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="70"/>
+      <c r="J59" s="70"/>
+      <c r="K59" s="70"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="59"/>
+      <c r="N59" s="59"/>
+    </row>
+    <row r="60" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="58"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="62"/>
+      <c r="F60" s="62"/>
+      <c r="G60" s="62"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70"/>
+      <c r="J60" s="70"/>
+      <c r="K60" s="70"/>
+      <c r="L60" s="59"/>
+      <c r="M60" s="59"/>
+      <c r="N60" s="59"/>
+    </row>
+    <row r="61" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="58"/>
+      <c r="B61" s="63"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="70"/>
+      <c r="I61" s="70"/>
+      <c r="J61" s="70"/>
+      <c r="K61" s="70"/>
+      <c r="L61" s="58"/>
+      <c r="M61" s="58"/>
+      <c r="N61" s="58"/>
+    </row>
+    <row r="62" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="58"/>
+      <c r="B62" s="63"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="70"/>
+      <c r="K62" s="70"/>
+      <c r="L62" s="58"/>
+      <c r="M62" s="58"/>
+      <c r="N62" s="58"/>
+    </row>
+    <row r="63" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="58"/>
+      <c r="B63" s="63"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="63"/>
+      <c r="F63" s="63"/>
+      <c r="G63" s="63"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
+      <c r="J63" s="70"/>
+      <c r="K63" s="70"/>
+      <c r="L63" s="58"/>
+      <c r="M63" s="58"/>
+      <c r="N63" s="58"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
@@ -5068,11 +5141,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="20.6640625" style="56"/>
+    <col min="1" max="1" width="10.5" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="20.6640625" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -5291,53 +5364,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" style="60" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="60" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="60" bestFit="1" customWidth="1"/>
-    <col min="7" max="251" width="12" style="62" customWidth="1"/>
-    <col min="252" max="16384" width="9.33203125" style="62"/>
+    <col min="1" max="1" width="12.83203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="58" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="251" width="12" style="60" customWidth="1"/>
+    <col min="252" max="16384" width="9.33203125" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:6" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="46" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44">
+    <row r="2" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="42">
         <f t="shared" ref="A2:A24" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44">
+    <row r="3" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="42">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44">
+    <row r="4" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="42">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47">
+    <row r="5" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="45">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -5345,8 +5418,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47">
+    <row r="6" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="45">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -5358,8 +5431,8 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="47">
+    <row r="7" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="45">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -5367,8 +5440,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47">
+    <row r="8" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="45">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -5380,8 +5453,8 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="47">
+    <row r="9" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="45">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -5393,8 +5466,8 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="47">
+    <row r="10" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="45">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -5406,8 +5479,8 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="47">
+    <row r="11" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="45">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -5419,8 +5492,8 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47">
+    <row r="12" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="45">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -5428,8 +5501,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="47">
+    <row r="13" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="45">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -5437,16 +5510,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="47">
+    <row r="14" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="45">
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="47">
+    <row r="15" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="45">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -5454,8 +5527,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="47">
+    <row r="16" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="45">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -5467,8 +5540,8 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="47">
+    <row r="17" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="45">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -5476,8 +5549,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="47">
+    <row r="18" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="45">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -5489,8 +5562,8 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="47">
+    <row r="19" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="45">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -5502,8 +5575,8 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="47">
+    <row r="20" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="45">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -5515,8 +5588,8 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="47">
+    <row r="21" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="45">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -5528,8 +5601,8 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="47">
+    <row r="22" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="45">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -5541,8 +5614,8 @@
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="47">
+    <row r="23" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="45">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -5554,8 +5627,8 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:6" s="58" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="47">
+    <row r="24" spans="1:6" s="56" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="45">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -5567,229 +5640,229 @@
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-    </row>
-    <row r="26" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-    </row>
-    <row r="27" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-    </row>
-    <row r="28" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-    </row>
-    <row r="29" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-    </row>
-    <row r="30" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="60"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="61"/>
-    </row>
-    <row r="31" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="60"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-    </row>
-    <row r="32" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="60"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-    </row>
-    <row r="33" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="60"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-    </row>
-    <row r="34" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-    </row>
-    <row r="35" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-    </row>
-    <row r="36" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
-    </row>
-    <row r="37" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-    </row>
-    <row r="38" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="60"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
-      <c r="F38" s="61"/>
-    </row>
-    <row r="39" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="60"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="61"/>
-    </row>
-    <row r="40" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="60"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-    </row>
-    <row r="41" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="60"/>
-      <c r="B41" s="61"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-    </row>
-    <row r="42" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="60"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-    </row>
-    <row r="43" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="60"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
-    </row>
-    <row r="44" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="60"/>
-      <c r="B44" s="61"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-    </row>
-    <row r="45" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="60"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-    </row>
-    <row r="46" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="60"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-    </row>
-    <row r="47" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="60"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="61"/>
-    </row>
-    <row r="48" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="60"/>
-      <c r="B48" s="61"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
-    </row>
-    <row r="49" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="60"/>
-      <c r="B49" s="61"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-    </row>
-    <row r="50" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="60"/>
-      <c r="B50" s="60"/>
-      <c r="C50" s="60"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
-    </row>
-    <row r="51" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="60"/>
-      <c r="B51" s="60"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
-      <c r="F51" s="60"/>
-    </row>
-    <row r="52" spans="1:6" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="60"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="60"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="60"/>
-      <c r="F52" s="60"/>
+    <row r="25" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="58"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+    </row>
+    <row r="26" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="58"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+    </row>
+    <row r="27" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="58"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+    </row>
+    <row r="28" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="58"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+    </row>
+    <row r="29" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="58"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+    </row>
+    <row r="30" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="58"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+    </row>
+    <row r="31" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="58"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+    </row>
+    <row r="32" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="58"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+    </row>
+    <row r="33" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="58"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+    </row>
+    <row r="34" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="58"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+    </row>
+    <row r="35" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="58"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+    </row>
+    <row r="36" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="58"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+    </row>
+    <row r="37" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="58"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+    </row>
+    <row r="38" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="58"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="59"/>
+    </row>
+    <row r="39" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="58"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="59"/>
+    </row>
+    <row r="40" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="58"/>
+      <c r="B40" s="59"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+    </row>
+    <row r="41" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="58"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="59"/>
+    </row>
+    <row r="42" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="58"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+    </row>
+    <row r="43" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="58"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+    </row>
+    <row r="44" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="58"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+    </row>
+    <row r="45" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="58"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+    </row>
+    <row r="46" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="58"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+    </row>
+    <row r="47" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="58"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="59"/>
+    </row>
+    <row r="48" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="58"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+    </row>
+    <row r="49" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="58"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+    </row>
+    <row r="50" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="58"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+    </row>
+    <row r="51" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="58"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="58"/>
+      <c r="F51" s="58"/>
+    </row>
+    <row r="52" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="58"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="58"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>

</xml_diff>

<commit_message>
2015-09-15 18:00 UTC--300 NaldoDj (marinaldo/dot/jesus/at/blacktdn/dot/com)
</commit_message>
<xml_diff>
--- a/templates/office/excel/rh/pensao/CalculoPensao.xlsx
+++ b/templates/office/excel/rh/pensao/CalculoPensao.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionários" sheetId="1" r:id="rId1"/>
@@ -3372,8 +3372,8 @@
   </sheetPr>
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3595,11 +3595,11 @@
         <v>Nome do Funcionário 1</v>
       </c>
       <c r="C9" s="30">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="31" t="str">
         <f>VLOOKUP(C9,Eventos!A:B,2,FALSE)</f>
-        <v>Cadastrar</v>
+        <v>DSR</v>
       </c>
       <c r="E9" s="28">
         <v>32.909999999999997</v>
@@ -4860,7 +4860,7 @@
   </sheetPr>
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4935,7 +4935,7 @@
       </c>
       <c r="D2" s="1">
         <f ca="1">Table2[Somar Base IRRF]-Table2[Pensão]</f>
-        <v>2310.0806919359025</v>
+        <v>2310.0806919358943</v>
       </c>
       <c r="E2" s="2">
         <f ca="1">VLOOKUP(Table2[Base IRRF],Tabela9[[Faixa Inicial]:[Alíquota (%)]],3,TRUE)</f>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="G2" s="1">
         <f ca="1">Table2[Base IRRF]*Table2[% IRRF]-Table2[Dedução]</f>
-        <v>30.456051895192672</v>
+        <v>30.456051895192047</v>
       </c>
       <c r="H2" s="1">
         <f>SUMIFS(Lançamento!E2:E49,Lançamento!A2:A49,Table1[ID],Lançamento!G2:G49,1)</f>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="I2" s="1">
         <f ca="1">Table2[Somar Base Pensão]-Table2[IRRF]</f>
-        <v>3406.0839481048074</v>
+        <v>3406.0839481048079</v>
       </c>
       <c r="J2" s="2">
         <f>VLOOKUP(A2,Funcionários!A:C,3,FALSE)</f>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="K2" s="1">
         <f ca="1">Table2[Base Pensão]*Table2[% Pensão]</f>
-        <v>783.39930806410575</v>
+        <v>783.39930806410587</v>
       </c>
       <c r="L2" s="55"/>
     </row>

</xml_diff>